<commit_message>
Manje izmjene u studiji izvedivosti
</commit_message>
<xml_diff>
--- a/1. Prijedlog projekta/Studija Izvedivosti-Online Videoteka.xlsx
+++ b/1. Prijedlog projekta/Studija Izvedivosti-Online Videoteka.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26821"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\PIS-projekt\DZ01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="268" documentId="8_{AF68479A-833F-4CAF-801B-9613BFE1EB9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC2D19C9-2B89-4FB5-977B-148F868D8BC5}"/>
+  <xr:revisionPtr revIDLastSave="305" documentId="8_{AF68479A-833F-4CAF-801B-9613BFE1EB9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{60C13C46-2083-4584-8A59-17EB94A01BFE}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Analiza izvedivosti" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="62">
   <si>
     <t>Analiza izvedivosti</t>
   </si>
@@ -137,25 +137,22 @@
     <t>Ukupno</t>
   </si>
   <si>
-    <t>Projekt menadžer</t>
-  </si>
-  <si>
-    <t>Frontend Developer</t>
-  </si>
-  <si>
-    <t>Backend Developer</t>
-  </si>
-  <si>
-    <t>Grafički dizajner</t>
-  </si>
-  <si>
-    <t>Testni inženjer</t>
+    <t>Projektni koordinator</t>
+  </si>
+  <si>
+    <t>Upravitelj projekta</t>
+  </si>
+  <si>
+    <t>Analitičar sustava</t>
+  </si>
+  <si>
+    <t>Programer</t>
   </si>
   <si>
     <t>Administrator baze podataka</t>
   </si>
   <si>
-    <t>Pisac dokumentacije</t>
+    <t>26,25</t>
   </si>
   <si>
     <t>Edukacije</t>
@@ -1123,7 +1120,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1313,49 +1310,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1378,6 +1332,48 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1701,10 +1697,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" ht="60.75" thickBot="1">
-      <c r="A1" s="75" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="76"/>
+      <c r="A1" s="85" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="86"/>
       <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
@@ -1737,7 +1733,7 @@
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="96" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -1775,7 +1771,7 @@
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="78"/>
+      <c r="A3" s="88"/>
       <c r="B3" s="6" t="s">
         <v>13</v>
       </c>
@@ -1811,7 +1807,7 @@
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="78"/>
+      <c r="A4" s="88"/>
       <c r="B4" s="6" t="s">
         <v>14</v>
       </c>
@@ -1847,7 +1843,7 @@
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="87"/>
+      <c r="A5" s="97"/>
       <c r="B5" s="54" t="s">
         <v>15</v>
       </c>
@@ -1883,7 +1879,7 @@
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="87"/>
+      <c r="A6" s="97"/>
       <c r="B6" s="54" t="s">
         <v>16</v>
       </c>
@@ -1919,7 +1915,7 @@
       </c>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="79"/>
+      <c r="A7" s="89"/>
       <c r="B7" s="7" t="s">
         <v>17</v>
       </c>
@@ -1955,10 +1951,10 @@
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="80" t="s">
+      <c r="A8" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="81"/>
+      <c r="B8" s="91"/>
       <c r="C8" s="37">
         <f>AVERAGE(C2:C7)</f>
         <v>0.83333333333333337</v>
@@ -2001,7 +1997,7 @@
       </c>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="86" t="s">
+      <c r="A9" s="96" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -2039,7 +2035,7 @@
       </c>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="78"/>
+      <c r="A10" s="88"/>
       <c r="B10" s="6" t="s">
         <v>13</v>
       </c>
@@ -2075,7 +2071,7 @@
       </c>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="78"/>
+      <c r="A11" s="88"/>
       <c r="B11" s="6" t="s">
         <v>14</v>
       </c>
@@ -2111,7 +2107,7 @@
       </c>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="87"/>
+      <c r="A12" s="97"/>
       <c r="B12" s="54" t="s">
         <v>15</v>
       </c>
@@ -2147,7 +2143,7 @@
       </c>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="87"/>
+      <c r="A13" s="97"/>
       <c r="B13" s="54" t="s">
         <v>16</v>
       </c>
@@ -2183,7 +2179,7 @@
       </c>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="79"/>
+      <c r="A14" s="89"/>
       <c r="B14" s="7" t="s">
         <v>17</v>
       </c>
@@ -2219,10 +2215,10 @@
       </c>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="82" t="s">
+      <c r="A15" s="92" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="83"/>
+      <c r="B15" s="93"/>
       <c r="C15" s="37">
         <f>AVERAGE(C9:C14)</f>
         <v>1.3333333333333333</v>
@@ -2265,7 +2261,7 @@
       </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="86" t="s">
+      <c r="A16" s="96" t="s">
         <v>20</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -2303,7 +2299,7 @@
       </c>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="78"/>
+      <c r="A17" s="88"/>
       <c r="B17" s="6" t="s">
         <v>13</v>
       </c>
@@ -2339,7 +2335,7 @@
       </c>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="78"/>
+      <c r="A18" s="88"/>
       <c r="B18" s="6" t="s">
         <v>14</v>
       </c>
@@ -2375,7 +2371,7 @@
       </c>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="87"/>
+      <c r="A19" s="97"/>
       <c r="B19" s="54" t="s">
         <v>15</v>
       </c>
@@ -2411,7 +2407,7 @@
       </c>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="87"/>
+      <c r="A20" s="97"/>
       <c r="B20" s="54" t="s">
         <v>16</v>
       </c>
@@ -2447,7 +2443,7 @@
       </c>
     </row>
     <row r="21" spans="1:12">
-      <c r="A21" s="79"/>
+      <c r="A21" s="89"/>
       <c r="B21" s="7" t="s">
         <v>17</v>
       </c>
@@ -2483,10 +2479,10 @@
       </c>
     </row>
     <row r="22" spans="1:12">
-      <c r="A22" s="84" t="s">
+      <c r="A22" s="94" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="85"/>
+      <c r="B22" s="95"/>
       <c r="C22" s="37">
         <f>AVERAGE(C16:C21)</f>
         <v>2.8333333333333335</v>
@@ -2553,7 +2549,7 @@
       <c r="J24" s="1"/>
     </row>
     <row r="25" spans="1:12" ht="15" customHeight="1">
-      <c r="A25" s="77" t="s">
+      <c r="A25" s="87" t="s">
         <v>21</v>
       </c>
       <c r="B25" s="5" t="s">
@@ -2581,7 +2577,7 @@
       </c>
     </row>
     <row r="26" spans="1:12">
-      <c r="A26" s="78"/>
+      <c r="A26" s="88"/>
       <c r="B26" s="6" t="s">
         <v>24</v>
       </c>
@@ -2601,7 +2597,7 @@
       <c r="L26" s="57"/>
     </row>
     <row r="27" spans="1:12">
-      <c r="A27" s="79"/>
+      <c r="A27" s="89"/>
       <c r="B27" s="7" t="s">
         <v>25</v>
       </c>
@@ -2640,10 +2636,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2658,11 +2654,11 @@
       <c r="A1" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="99"/>
-      <c r="C1" s="99" t="s">
+      <c r="B1" s="84"/>
+      <c r="C1" s="84" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="99"/>
+      <c r="D1" s="84"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="20" t="s">
@@ -2691,11 +2687,11 @@
         <v>250</v>
       </c>
       <c r="C5" s="17">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="D5" s="18">
-        <f>B5*C5</f>
-        <v>10000</v>
+        <f>6500</f>
+        <v>6500</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2706,11 +2702,10 @@
         <v>250</v>
       </c>
       <c r="C6" s="12">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D6" s="3">
-        <f t="shared" ref="D6:D13" si="0">B6*C6</f>
-        <v>7500</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -2721,11 +2716,10 @@
         <v>250</v>
       </c>
       <c r="C7" s="12">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D7" s="3">
-        <f t="shared" si="0"/>
-        <v>7500</v>
+        <v>8000</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -2739,7 +2733,6 @@
         <v>25</v>
       </c>
       <c r="D8" s="3">
-        <f t="shared" si="0"/>
         <v>5000</v>
       </c>
     </row>
@@ -2748,45 +2741,26 @@
         <v>37</v>
       </c>
       <c r="B9" s="36">
-        <v>150</v>
-      </c>
-      <c r="C9" s="14">
-        <v>25</v>
+        <v>160</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>38</v>
       </c>
       <c r="D9" s="15">
-        <f>B9*C9</f>
-        <v>3750</v>
+        <v>4200</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="48" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="12">
-        <v>180</v>
-      </c>
-      <c r="C10" s="32">
-        <v>25</v>
-      </c>
-      <c r="D10" s="3">
-        <f>B10*C10</f>
-        <v>4500</v>
-      </c>
+      <c r="A10" s="48"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" s="19">
-        <v>130</v>
-      </c>
-      <c r="C11" s="28">
-        <v>10</v>
-      </c>
-      <c r="D11" s="4">
-        <f>B11*C11</f>
-        <v>1300</v>
-      </c>
+      <c r="A11" s="47"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="4"/>
     </row>
     <row r="13" spans="1:4">
       <c r="C13"/>
@@ -2794,7 +2768,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B14" s="25"/>
       <c r="C14" s="25"/>
@@ -2802,13 +2776,13 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="26" t="s">
+      <c r="C15" s="21" t="s">
         <v>42</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>43</v>
       </c>
       <c r="D15" s="22" t="s">
         <v>32</v>
@@ -2816,7 +2790,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B16" s="27">
         <v>20</v>
@@ -2829,9 +2803,9 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:7">
       <c r="A17" s="31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B17" s="28">
         <v>15</v>
@@ -2844,9 +2818,9 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:7">
       <c r="A18" s="31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B18" s="28">
         <v>2</v>
@@ -2859,9 +2833,9 @@
         <v>400</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:7">
       <c r="A19" s="49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B19" s="51">
         <v>3</v>
@@ -2872,29 +2846,28 @@
       <c r="D19" s="50">
         <v>1050</v>
       </c>
-      <c r="K19" s="89"/>
-    </row>
-    <row r="21" spans="1:11">
-      <c r="G21" s="94"/>
-    </row>
-    <row r="22" spans="1:11">
+    </row>
+    <row r="21" spans="1:7">
+      <c r="G21" s="79"/>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" s="20" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" s="29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B23" s="34"/>
       <c r="C23" s="23"/>
       <c r="D23" s="22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="30" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11">
-      <c r="A24" s="30" t="s">
-        <v>50</v>
       </c>
       <c r="B24" s="27"/>
       <c r="C24" s="17"/>
@@ -2902,9 +2875,9 @@
         <v>300</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:7">
       <c r="A25" s="31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B25" s="28"/>
       <c r="C25" s="19"/>
@@ -2912,9 +2885,9 @@
         <v>200</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:7">
       <c r="A26" s="49" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B26" s="51"/>
       <c r="C26" s="34"/>
@@ -2922,28 +2895,28 @@
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:7">
       <c r="A29" s="20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="26" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="30" spans="1:11">
-      <c r="A30" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="B30" s="26" t="s">
+      <c r="C30" s="21" t="s">
         <v>54</v>
-      </c>
-      <c r="C30" s="21" t="s">
-        <v>55</v>
       </c>
       <c r="D30" s="22" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:7">
       <c r="A31" s="33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B31" s="44">
         <v>5</v>
@@ -2956,9 +2929,9 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:7">
       <c r="A32" s="33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B32" s="44">
         <v>30</v>
@@ -2973,7 +2946,7 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B33" s="32">
         <v>30</v>
@@ -2982,13 +2955,13 @@
         <v>300</v>
       </c>
       <c r="D33" s="3">
-        <f t="shared" ref="D33:D35" si="1">B33*C33</f>
+        <f t="shared" ref="D33:D35" si="0">B33*C33</f>
         <v>9000</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B34" s="28">
         <v>30</v>
@@ -2997,36 +2970,36 @@
         <v>500</v>
       </c>
       <c r="D34" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>15000</v>
       </c>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="90" t="s">
+      <c r="A35" s="75" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" s="76">
+        <v>1</v>
+      </c>
+      <c r="C35" s="77">
+        <v>8000</v>
+      </c>
+      <c r="D35" s="78">
+        <f t="shared" si="0"/>
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="80" t="s">
         <v>60</v>
       </c>
-      <c r="B35" s="91">
-        <v>1</v>
-      </c>
-      <c r="C35" s="92">
-        <v>8000</v>
-      </c>
-      <c r="D35" s="93">
-        <f t="shared" si="1"/>
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="95" t="s">
-        <v>61</v>
-      </c>
-      <c r="B36" s="96">
-        <v>1</v>
-      </c>
-      <c r="C36" s="97">
+      <c r="B36" s="81">
+        <v>1</v>
+      </c>
+      <c r="C36" s="82">
         <v>10000</v>
       </c>
-      <c r="D36" s="98">
+      <c r="D36" s="83">
         <v>10000</v>
       </c>
     </row>
@@ -3036,14 +3009,14 @@
       <c r="D37"/>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="80" t="s">
-        <v>62</v>
-      </c>
-      <c r="B39" s="88"/>
-      <c r="C39" s="81"/>
+      <c r="A39" s="90" t="s">
+        <v>61</v>
+      </c>
+      <c r="B39" s="98"/>
+      <c r="C39" s="91"/>
       <c r="D39" s="42">
         <f>SUM(D1:D38)</f>
-        <v>157850</v>
+        <v>152000</v>
       </c>
     </row>
   </sheetData>
@@ -3068,23 +3041,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <Komentar xmlns="d34a4129-52ec-4ee5-bc77-23d8e5f94cfd" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101007AFC1106DB8A04488E866355A5CEB218" ma:contentTypeVersion="2" ma:contentTypeDescription="Stvaranje novog dokumenta." ma:contentTypeScope="" ma:versionID="cf5653b097a0dc1db313e4d0258d9f51">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d34a4129-52ec-4ee5-bc77-23d8e5f94cfd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3c81d14dc3ad95f274f0f0999b8e60d5" ns2:_="">
     <xsd:import namespace="d34a4129-52ec-4ee5-bc77-23d8e5f94cfd"/>
@@ -3144,8 +3100,25 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <Komentar xmlns="d34a4129-52ec-4ee5-bc77-23d8e5f94cfd" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5758EF3-F7D3-4420-8E13-AF1AC80FD17D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{033D9B50-45AF-432E-87DC-2944701B1988}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3153,5 +3126,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{033D9B50-45AF-432E-87DC-2944701B1988}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5758EF3-F7D3-4420-8E13-AF1AC80FD17D}"/>
 </file>
</xml_diff>